<commit_message>
Data were correct the first time around
</commit_message>
<xml_diff>
--- a/Data/TrappingSimulation.xlsx
+++ b/Data/TrappingSimulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Wild dogs\Forensics\Field work\Scat searches\TrappingSimulationAnalysis\WDTrappingAnalysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BF4780-3E69-4AE3-9E55-A3D0FB0E7B67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F11130-A99F-47F9-8595-3056C726845F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30885" yWindow="1005" windowWidth="26145" windowHeight="15810" activeTab="3" xr2:uid="{2710E8AD-00DC-40F3-B0B0-9BC2CF75077C}"/>
+    <workbookView xWindow="31455" yWindow="2190" windowWidth="26145" windowHeight="15810" activeTab="3" xr2:uid="{2710E8AD-00DC-40F3-B0B0-9BC2CF75077C}"/>
   </bookViews>
   <sheets>
     <sheet name="Trap" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="217">
   <si>
     <t xml:space="preserve">Day 1 </t>
   </si>
@@ -14753,7 +14753,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="A20" sqref="A20:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15645,49 +15645,18 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>43419</v>
-      </c>
-      <c r="B20" t="s">
-        <v>204</v>
-      </c>
-      <c r="C20" t="s">
-        <v>187</v>
-      </c>
-      <c r="D20" t="s">
-        <v>187</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="F20" s="12">
-        <f>VLOOKUP($B20,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
-        <v>442776.59759999998</v>
-      </c>
-      <c r="G20" s="12">
-        <f>VLOOKUP($B20,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
-        <v>5899051.3799999999</v>
-      </c>
-      <c r="H20" s="22">
-        <v>17.196313858032227</v>
-      </c>
-      <c r="I20" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="L20" s="23">
-        <v>11</v>
-      </c>
-      <c r="M20" s="12" t="e">
-        <f>VLOOKUP(B20,'[2]Purity Results'!$A$2:$E$47,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N20" s="12">
-        <f>IF(ISERROR(VLOOKUP(B20,[2]clean_8mism_all!$A$3:$D$58,4,FALSE)),VLOOKUP(B20,[2]clean_8mism_all!$B$3:$D$58,3,FALSE),VLOOKUP(B20,[2]clean_8mism_all!$A$3:$D$58,4,FALSE))</f>
-        <v>45</v>
-      </c>
+      <c r="A20" s="8"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="13"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N19" xr:uid="{B10F9094-E95D-4553-8907-615241E346AF}"/>

</xml_diff>

<commit_message>
updated coords for scats
</commit_message>
<xml_diff>
--- a/Data/TrappingSimulation.xlsx
+++ b/Data/TrappingSimulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Wild dogs\Forensics\Field work\Scat searches\TrappingSimulationAnalysis\WDTrappingAnalysis\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Dropbox\Wild dogs\Forensics\Field work\Scat searches\TrappingSimulationAnalysis\WDTrappingAnalysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F11130-A99F-47F9-8595-3056C726845F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD783003-4BD1-4416-8051-E41D5CDFC46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31455" yWindow="2190" windowWidth="26145" windowHeight="15810" activeTab="3" xr2:uid="{2710E8AD-00DC-40F3-B0B0-9BC2CF75077C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{2710E8AD-00DC-40F3-B0B0-9BC2CF75077C}"/>
   </bookViews>
   <sheets>
     <sheet name="Trap" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -60,24 +62,6 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={7C8EE94D-1E23-477C-ACA5-9A8619D6FA0D}</author>
-  </authors>
-  <commentList>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{7C8EE94D-1E23-477C-ACA5-9A8619D6FA0D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    see notes</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="217">
   <si>
@@ -729,7 +713,7 @@
     <t>B07 was shot the day before scat search. The scat was very fresh, CT value was very low so estimated that it wouldn't be older than two days</t>
   </si>
   <si>
-    <t>coords are made up, waiting for Luke (canidae) to get back to me about this</t>
+    <t>coords are now correct, see email from Luke (canidae) 01 Nov 2019</t>
   </si>
 </sst>
 </file>
@@ -812,7 +796,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -875,7 +859,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3827,6 +3810,84 @@
             <v>Mansfield</v>
           </cell>
         </row>
+        <row r="115">
+          <cell r="A115" t="str">
+            <v>WDJ42</v>
+          </cell>
+          <cell r="B115">
+            <v>43419</v>
+          </cell>
+          <cell r="C115" t="str">
+            <v>FOX</v>
+          </cell>
+          <cell r="D115" t="str">
+            <v>fur, bones</v>
+          </cell>
+          <cell r="E115" t="str">
+            <v>dry</v>
+          </cell>
+          <cell r="F115">
+            <v>438395.11678785097</v>
+          </cell>
+          <cell r="G115">
+            <v>5899590.0553073203</v>
+          </cell>
+          <cell r="H115" t="str">
+            <v>Mansfield</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="A116" t="str">
+            <v>WDJ43</v>
+          </cell>
+          <cell r="B116">
+            <v>43419</v>
+          </cell>
+          <cell r="C116" t="str">
+            <v>FOX</v>
+          </cell>
+          <cell r="D116" t="str">
+            <v>bugs</v>
+          </cell>
+          <cell r="E116" t="str">
+            <v>dry</v>
+          </cell>
+          <cell r="F116">
+            <v>437374.18468051997</v>
+          </cell>
+          <cell r="G116">
+            <v>5898841.0174039202</v>
+          </cell>
+          <cell r="H116" t="str">
+            <v>Mansfield</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="A117" t="str">
+            <v>WDN35</v>
+          </cell>
+          <cell r="B117">
+            <v>43419</v>
+          </cell>
+          <cell r="C117" t="str">
+            <v>WD</v>
+          </cell>
+          <cell r="D117" t="str">
+            <v>fur</v>
+          </cell>
+          <cell r="E117" t="str">
+            <v>fresh</v>
+          </cell>
+          <cell r="F117">
+            <v>441768.414472214</v>
+          </cell>
+          <cell r="G117">
+            <v>5904571.1350657903</v>
+          </cell>
+          <cell r="H117" t="str">
+            <v>Mansfield</v>
+          </cell>
+        </row>
       </sheetData>
     </sheetDataSet>
   </externalBook>
@@ -5422,7 +5483,6 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="carlo pacioni" id="{29244497-69F9-43F0-B30F-82993030FDD9}" userId="1b3ed7e66be81e2c" providerId="Windows Live"/>
   <person displayName="Carlo Pacioni (DELWP)" id="{2AC313B9-2D10-486A-914A-1B3091D7E81A}" userId="S::carlo.pacioni@delwp.vic.gov.au::825da1f5-54c0-44f1-8ee3-46f5ec2d5dff" providerId="AD"/>
 </personList>
 </file>
@@ -5730,14 +5790,6 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F10" dT="2019-11-03T23:46:10.64" personId="{2AC313B9-2D10-486A-914A-1B3091D7E81A}" id="{7C8EE94D-1E23-477C-ACA5-9A8619D6FA0D}">
-    <text>see notes</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB7B390-8F80-4E96-A178-C77719E95CF9}">
   <dimension ref="A1:CA110"/>
@@ -5748,20 +5800,20 @@
       <selection pane="topRight" activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="17" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="48" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="49" max="57" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="48" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="57" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="60" max="78" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="79" max="16384" width="8.7109375" style="2"/>
+    <col min="79" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
@@ -5940,7 +5992,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>211</v>
       </c>
@@ -6138,7 +6190,7 @@
       <c r="BY2" s="4"/>
       <c r="BZ2" s="4"/>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -6336,7 +6388,7 @@
       <c r="BY3" s="5"/>
       <c r="BZ3" s="5"/>
     </row>
-    <row r="4" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -6534,7 +6586,7 @@
       <c r="BY4" s="5"/>
       <c r="BZ4" s="5"/>
     </row>
-    <row r="5" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -6713,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -6892,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -7071,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -7261,7 +7313,7 @@
       <c r="BQ8" s="5"/>
       <c r="BR8" s="5"/>
     </row>
-    <row r="9" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -7451,7 +7503,7 @@
       <c r="BQ9" s="5"/>
       <c r="BR9" s="5"/>
     </row>
-    <row r="10" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -7650,7 +7702,7 @@
       <c r="BZ10" s="5"/>
       <c r="CA10" s="5"/>
     </row>
-    <row r="11" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -7848,7 +7900,7 @@
       <c r="BY11" s="5"/>
       <c r="BZ11" s="5"/>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -8046,7 +8098,7 @@
       <c r="BY12" s="5"/>
       <c r="BZ12" s="5"/>
     </row>
-    <row r="13" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -8244,7 +8296,7 @@
       <c r="BY13" s="5"/>
       <c r="BZ13" s="5"/>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -8442,7 +8494,7 @@
       <c r="BY14" s="5"/>
       <c r="BZ14" s="5"/>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -8640,7 +8692,7 @@
       <c r="BY15" s="5"/>
       <c r="BZ15" s="5"/>
     </row>
-    <row r="16" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -8838,7 +8890,7 @@
       <c r="BY16" s="5"/>
       <c r="BZ16" s="5"/>
     </row>
-    <row r="17" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -9036,7 +9088,7 @@
       <c r="BY17" s="5"/>
       <c r="BZ17" s="5"/>
     </row>
-    <row r="18" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -9215,7 +9267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -9394,7 +9446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -9423,7 +9475,7 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
     </row>
-    <row r="21" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -9452,7 +9504,7 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
     </row>
-    <row r="22" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -9481,7 +9533,7 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
     </row>
-    <row r="23" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -9510,7 +9562,7 @@
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
     </row>
-    <row r="24" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -9539,7 +9591,7 @@
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
     </row>
-    <row r="25" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -9568,7 +9620,7 @@
       <c r="Z25" s="5"/>
       <c r="AA25" s="5"/>
     </row>
-    <row r="26" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -9597,7 +9649,7 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
     </row>
-    <row r="27" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -9626,7 +9678,7 @@
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
     </row>
-    <row r="28" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -9655,7 +9707,7 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="5"/>
     </row>
-    <row r="29" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -9684,7 +9736,7 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="5"/>
     </row>
-    <row r="30" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -9713,7 +9765,7 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
     </row>
-    <row r="31" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -9742,7 +9794,7 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="5"/>
     </row>
-    <row r="32" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -9771,7 +9823,7 @@
       <c r="Z32" s="5"/>
       <c r="AA32" s="5"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -9800,7 +9852,7 @@
       <c r="Z33" s="5"/>
       <c r="AA33" s="5"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -9829,7 +9881,7 @@
       <c r="Z34" s="5"/>
       <c r="AA34" s="5"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -9858,7 +9910,7 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -9887,7 +9939,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -9916,7 +9968,7 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -9945,7 +9997,7 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -9974,7 +10026,7 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -10003,7 +10055,7 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -10032,7 +10084,7 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -10061,7 +10113,7 @@
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -10090,7 +10142,7 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -10119,7 +10171,7 @@
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -10148,7 +10200,7 @@
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -10177,7 +10229,7 @@
       <c r="Z46" s="5"/>
       <c r="AA46" s="5"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -10206,7 +10258,7 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -10235,7 +10287,7 @@
       <c r="Z48" s="5"/>
       <c r="AA48" s="5"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -10264,7 +10316,7 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -10293,7 +10345,7 @@
       <c r="Z50" s="5"/>
       <c r="AA50" s="5"/>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -10322,7 +10374,7 @@
       <c r="Z51" s="5"/>
       <c r="AA51" s="5"/>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -10351,7 +10403,7 @@
       <c r="Z52" s="5"/>
       <c r="AA52" s="5"/>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -10380,7 +10432,7 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -10409,7 +10461,7 @@
       <c r="Z54" s="5"/>
       <c r="AA54" s="5"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -10438,7 +10490,7 @@
       <c r="Z55" s="5"/>
       <c r="AA55" s="5"/>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -10467,7 +10519,7 @@
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -10496,7 +10548,7 @@
       <c r="Z57" s="5"/>
       <c r="AA57" s="5"/>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -10525,7 +10577,7 @@
       <c r="Z58" s="5"/>
       <c r="AA58" s="5"/>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -10554,7 +10606,7 @@
       <c r="Z59" s="5"/>
       <c r="AA59" s="5"/>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -10583,7 +10635,7 @@
       <c r="Z60" s="5"/>
       <c r="AA60" s="5"/>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -10612,7 +10664,7 @@
       <c r="Z61" s="5"/>
       <c r="AA61" s="5"/>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A62" s="3"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -10641,7 +10693,7 @@
       <c r="Z62" s="5"/>
       <c r="AA62" s="5"/>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -10670,7 +10722,7 @@
       <c r="Z63" s="5"/>
       <c r="AA63" s="5"/>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -10699,7 +10751,7 @@
       <c r="Z64" s="5"/>
       <c r="AA64" s="5"/>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -10728,7 +10780,7 @@
       <c r="Z65" s="5"/>
       <c r="AA65" s="5"/>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -10757,7 +10809,7 @@
       <c r="Z66" s="5"/>
       <c r="AA66" s="5"/>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -10786,7 +10838,7 @@
       <c r="Z67" s="5"/>
       <c r="AA67" s="5"/>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -10815,7 +10867,7 @@
       <c r="Z68" s="5"/>
       <c r="AA68" s="5"/>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -10844,7 +10896,7 @@
       <c r="Z69" s="5"/>
       <c r="AA69" s="5"/>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -10873,7 +10925,7 @@
       <c r="Z70" s="5"/>
       <c r="AA70" s="5"/>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -10902,7 +10954,7 @@
       <c r="Z71" s="5"/>
       <c r="AA71" s="5"/>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A72" s="3"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -10931,7 +10983,7 @@
       <c r="Z72" s="5"/>
       <c r="AA72" s="5"/>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A73" s="3"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
@@ -10960,7 +11012,7 @@
       <c r="Z73" s="5"/>
       <c r="AA73" s="5"/>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A74" s="3"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -10989,7 +11041,7 @@
       <c r="Z74" s="5"/>
       <c r="AA74" s="5"/>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A75" s="3"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
@@ -11018,7 +11070,7 @@
       <c r="Z75" s="5"/>
       <c r="AA75" s="5"/>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A76" s="3"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -11047,7 +11099,7 @@
       <c r="Z76" s="5"/>
       <c r="AA76" s="5"/>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A77" s="3"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
@@ -11076,7 +11128,7 @@
       <c r="Z77" s="5"/>
       <c r="AA77" s="5"/>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A78" s="3"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
@@ -11105,7 +11157,7 @@
       <c r="Z78" s="5"/>
       <c r="AA78" s="5"/>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A79" s="3"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -11134,7 +11186,7 @@
       <c r="Z79" s="5"/>
       <c r="AA79" s="5"/>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A80" s="3"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
@@ -11163,7 +11215,7 @@
       <c r="Z80" s="5"/>
       <c r="AA80" s="5"/>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A81" s="3"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -11192,7 +11244,7 @@
       <c r="Z81" s="5"/>
       <c r="AA81" s="5"/>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A82" s="3"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -11221,7 +11273,7 @@
       <c r="Z82" s="5"/>
       <c r="AA82" s="5"/>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A83" s="3"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -11250,7 +11302,7 @@
       <c r="Z83" s="5"/>
       <c r="AA83" s="5"/>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A84" s="3"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -11279,7 +11331,7 @@
       <c r="Z84" s="5"/>
       <c r="AA84" s="5"/>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A85" s="3"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -11308,7 +11360,7 @@
       <c r="Z85" s="5"/>
       <c r="AA85" s="5"/>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A86" s="3"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -11337,7 +11389,7 @@
       <c r="Z86" s="5"/>
       <c r="AA86" s="5"/>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A87" s="3"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -11366,7 +11418,7 @@
       <c r="Z87" s="5"/>
       <c r="AA87" s="5"/>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A88" s="3"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -11395,7 +11447,7 @@
       <c r="Z88" s="5"/>
       <c r="AA88" s="5"/>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A89" s="3"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -11424,7 +11476,7 @@
       <c r="Z89" s="5"/>
       <c r="AA89" s="5"/>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A90" s="3"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -11453,7 +11505,7 @@
       <c r="Z90" s="5"/>
       <c r="AA90" s="5"/>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A91" s="3"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -11482,7 +11534,7 @@
       <c r="Z91" s="5"/>
       <c r="AA91" s="5"/>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A92" s="3"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -11511,7 +11563,7 @@
       <c r="Z92" s="5"/>
       <c r="AA92" s="5"/>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A93" s="3"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -11540,7 +11592,7 @@
       <c r="Z93" s="5"/>
       <c r="AA93" s="5"/>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A94" s="3"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -11569,7 +11621,7 @@
       <c r="Z94" s="5"/>
       <c r="AA94" s="5"/>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A95" s="3"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
@@ -11598,7 +11650,7 @@
       <c r="Z95" s="5"/>
       <c r="AA95" s="5"/>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A96" s="3"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
@@ -11627,7 +11679,7 @@
       <c r="Z96" s="5"/>
       <c r="AA96" s="5"/>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A97" s="3"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
@@ -11656,7 +11708,7 @@
       <c r="Z97" s="5"/>
       <c r="AA97" s="5"/>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A98" s="3"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
@@ -11685,7 +11737,7 @@
       <c r="Z98" s="5"/>
       <c r="AA98" s="5"/>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A99" s="3"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
@@ -11714,7 +11766,7 @@
       <c r="Z99" s="5"/>
       <c r="AA99" s="5"/>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A100" s="3"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
@@ -11743,7 +11795,7 @@
       <c r="Z100" s="5"/>
       <c r="AA100" s="5"/>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A101" s="3"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
@@ -11772,7 +11824,7 @@
       <c r="Z101" s="5"/>
       <c r="AA101" s="5"/>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A102" s="3"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -11801,7 +11853,7 @@
       <c r="Z102" s="5"/>
       <c r="AA102" s="5"/>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A103" s="3"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
@@ -11830,7 +11882,7 @@
       <c r="Z103" s="5"/>
       <c r="AA103" s="5"/>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A104" s="3"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
@@ -11859,7 +11911,7 @@
       <c r="Z104" s="5"/>
       <c r="AA104" s="5"/>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A105" s="3"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
@@ -11888,7 +11940,7 @@
       <c r="Z105" s="5"/>
       <c r="AA105" s="5"/>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A106" s="3"/>
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
@@ -11917,7 +11969,7 @@
       <c r="Z106" s="5"/>
       <c r="AA106" s="5"/>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A107" s="3"/>
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
@@ -11946,7 +11998,7 @@
       <c r="Z107" s="5"/>
       <c r="AA107" s="5"/>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A108" s="3"/>
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
@@ -11975,7 +12027,7 @@
       <c r="Z108" s="5"/>
       <c r="AA108" s="5"/>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A109" s="3"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
@@ -12004,7 +12056,7 @@
       <c r="Z109" s="5"/>
       <c r="AA109" s="5"/>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -12056,14 +12108,14 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>214</v>
       </c>
@@ -12083,7 +12135,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>172</v>
       </c>
@@ -12103,7 +12155,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>170</v>
       </c>
@@ -12133,19 +12185,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC74EFC9-D6BB-4BDC-9373-237FF6938D88}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -12174,7 +12226,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -12200,7 +12252,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -12226,7 +12278,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -12252,7 +12304,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -12278,7 +12330,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -12304,7 +12356,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -12330,7 +12382,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -12356,7 +12408,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -12382,7 +12434,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>78</v>
       </c>
@@ -12408,7 +12460,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -12434,7 +12486,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -12460,7 +12512,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -12486,7 +12538,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -12512,7 +12564,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -12538,7 +12590,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -12564,7 +12616,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -12590,7 +12642,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -12616,7 +12668,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -12642,7 +12694,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -12668,7 +12720,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -12694,7 +12746,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -12720,7 +12772,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -12746,7 +12798,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -12772,7 +12824,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -12798,7 +12850,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -12824,7 +12876,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -12850,7 +12902,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>96</v>
       </c>
@@ -12876,7 +12928,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -12902,7 +12954,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -12928,7 +12980,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -12954,7 +13006,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -12980,7 +13032,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -13006,7 +13058,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -13032,7 +13084,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -13058,7 +13110,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -13084,7 +13136,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -13110,7 +13162,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>107</v>
       </c>
@@ -13136,7 +13188,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -13162,7 +13214,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>109</v>
       </c>
@@ -13188,7 +13240,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>110</v>
       </c>
@@ -13214,7 +13266,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -13240,7 +13292,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>112</v>
       </c>
@@ -13263,7 +13315,7 @@
         <v>-36.979722219999999</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -13289,7 +13341,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -13312,7 +13364,7 @@
         <v>-36.979444399999998</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>115</v>
       </c>
@@ -13338,7 +13390,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>116</v>
       </c>
@@ -13364,7 +13416,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>117</v>
       </c>
@@ -13390,7 +13442,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>118</v>
       </c>
@@ -13416,7 +13468,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>119</v>
       </c>
@@ -13442,7 +13494,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>120</v>
       </c>
@@ -13468,7 +13520,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>121</v>
       </c>
@@ -13494,7 +13546,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -13520,7 +13572,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>123</v>
       </c>
@@ -13546,7 +13598,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>124</v>
       </c>
@@ -13572,7 +13624,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>125</v>
       </c>
@@ -13598,7 +13650,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>126</v>
       </c>
@@ -13624,7 +13676,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>127</v>
       </c>
@@ -13650,7 +13702,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>128</v>
       </c>
@@ -13676,7 +13728,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -13702,7 +13754,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>130</v>
       </c>
@@ -13728,7 +13780,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -13754,7 +13806,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>132</v>
       </c>
@@ -13780,7 +13832,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -13806,7 +13858,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -13832,7 +13884,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>135</v>
       </c>
@@ -13858,7 +13910,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -13884,7 +13936,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -13910,7 +13962,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -13936,7 +13988,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>139</v>
       </c>
@@ -13962,7 +14014,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -13988,7 +14040,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>141</v>
       </c>
@@ -14014,7 +14066,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -14040,7 +14092,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -14066,7 +14118,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>144</v>
       </c>
@@ -14092,7 +14144,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>145</v>
       </c>
@@ -14118,7 +14170,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -14144,7 +14196,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -14170,7 +14222,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>148</v>
       </c>
@@ -14196,7 +14248,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -14222,7 +14274,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>150</v>
       </c>
@@ -14248,7 +14300,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -14274,7 +14326,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>152</v>
       </c>
@@ -14300,7 +14352,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>153</v>
       </c>
@@ -14326,7 +14378,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>154</v>
       </c>
@@ -14352,7 +14404,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>155</v>
       </c>
@@ -14378,7 +14430,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>156</v>
       </c>
@@ -14404,7 +14456,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>157</v>
       </c>
@@ -14430,7 +14482,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>158</v>
       </c>
@@ -14456,7 +14508,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>159</v>
       </c>
@@ -14482,7 +14534,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>160</v>
       </c>
@@ -14508,7 +14560,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>161</v>
       </c>
@@ -14534,7 +14586,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>162</v>
       </c>
@@ -14560,7 +14612,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>163</v>
       </c>
@@ -14586,7 +14638,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>164</v>
       </c>
@@ -14612,7 +14664,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>165</v>
       </c>
@@ -14638,7 +14690,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>166</v>
       </c>
@@ -14664,7 +14716,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>167</v>
       </c>
@@ -14690,7 +14742,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>168</v>
       </c>
@@ -14716,7 +14768,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>169</v>
       </c>
@@ -14749,32 +14801,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FCDAD8-3241-4B9B-A741-CC3F8E4D1679}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FCDAD8-3241-4B9B-A741-CC3F8E4D1679}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:N20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="23" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.140625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.1796875" style="15" customWidth="1"/>
     <col min="8" max="8" width="7" style="23" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="23" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" style="23" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" style="24" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="15"/>
+    <col min="9" max="9" width="6.453125" style="23" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" style="23" customWidth="1"/>
+    <col min="11" max="11" width="3.7265625" style="24" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1796875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>62</v>
       </c>
@@ -14818,7 +14870,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="20">
         <v>43418</v>
       </c>
@@ -14835,11 +14887,11 @@
         <v>188</v>
       </c>
       <c r="F2" s="12">
-        <f>VLOOKUP($B2,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B2,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>435925.8358</v>
       </c>
       <c r="G2" s="12">
-        <f>VLOOKUP($B2,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B2,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5901191.9179999996</v>
       </c>
       <c r="H2" s="21">
@@ -14864,7 +14916,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="20">
         <v>43418</v>
       </c>
@@ -14881,11 +14933,11 @@
         <v>188</v>
       </c>
       <c r="F3" s="12">
-        <f>VLOOKUP($B3,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B3,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>438042.52620000002</v>
       </c>
       <c r="G3" s="12">
-        <f>VLOOKUP($B3,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B3,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5902419.6100000003</v>
       </c>
       <c r="H3" s="21">
@@ -14910,7 +14962,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="20">
         <v>43418</v>
       </c>
@@ -14927,11 +14979,11 @@
         <v>188</v>
       </c>
       <c r="F4" s="12">
-        <f>VLOOKUP($B4,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B4,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>438782.36800000002</v>
       </c>
       <c r="G4" s="12">
-        <f>VLOOKUP($B4,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B4,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5901793.5149999997</v>
       </c>
       <c r="H4" s="21">
@@ -14956,7 +15008,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="20">
         <v>43418</v>
       </c>
@@ -14973,11 +15025,11 @@
         <v>188</v>
       </c>
       <c r="F5" s="12">
-        <f>VLOOKUP($B5,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B5,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>438969.98869999999</v>
       </c>
       <c r="G5" s="12">
-        <f>VLOOKUP($B5,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B5,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5901579.7560000001</v>
       </c>
       <c r="H5" s="22">
@@ -15002,7 +15054,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="20">
         <v>43418</v>
       </c>
@@ -15019,11 +15071,11 @@
         <v>188</v>
       </c>
       <c r="F6" s="12">
-        <f>VLOOKUP($B6,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B6,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>439137.49660000001</v>
       </c>
       <c r="G6" s="12">
-        <f>VLOOKUP($B6,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B6,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5901466.0269999998</v>
       </c>
       <c r="H6" s="22">
@@ -15048,7 +15100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="20">
         <v>43419</v>
       </c>
@@ -15065,11 +15117,11 @@
         <v>188</v>
       </c>
       <c r="F7" s="12">
-        <f>VLOOKUP($B7,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B7,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>442930.9</v>
       </c>
       <c r="G7" s="12">
-        <f>VLOOKUP($B7,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B7,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5899811.2570000002</v>
       </c>
       <c r="H7" s="22">
@@ -15094,7 +15146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="20">
         <v>43419</v>
       </c>
@@ -15111,11 +15163,11 @@
         <v>188</v>
       </c>
       <c r="F8" s="12">
-        <f>VLOOKUP($B8,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B8,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>442216.20159999997</v>
       </c>
       <c r="G8" s="12">
-        <f>VLOOKUP($B8,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B8,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5902061.8420000002</v>
       </c>
       <c r="H8" s="22">
@@ -15140,7 +15192,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>43419</v>
       </c>
@@ -15157,11 +15209,11 @@
         <v>188</v>
       </c>
       <c r="F9" s="12">
-        <f>VLOOKUP($B9,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B9,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>441920.86969999998</v>
       </c>
       <c r="G9" s="12">
-        <f>VLOOKUP($B9,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B9,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5902673.3190000001</v>
       </c>
       <c r="H9" s="22">
@@ -15186,7 +15238,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="20">
         <v>43419</v>
       </c>
@@ -15202,11 +15254,13 @@
       <c r="E10" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="F10" s="26">
-        <v>437132.65730000002</v>
-      </c>
-      <c r="G10" s="26">
-        <v>5902601.7280000001</v>
+      <c r="F10" s="12">
+        <f>VLOOKUP($B10,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
+        <v>438395.11678785097</v>
+      </c>
+      <c r="G10" s="12">
+        <f>VLOOKUP($B10,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
+        <v>5899590.0553073203</v>
       </c>
       <c r="H10" s="22">
         <v>18.566904067993164</v>
@@ -15230,7 +15284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="20">
         <v>43433</v>
       </c>
@@ -15247,11 +15301,11 @@
         <v>198</v>
       </c>
       <c r="F11" s="12">
-        <f>VLOOKUP($B11,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B11,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>560628.65159999998</v>
       </c>
       <c r="G11" s="12">
-        <f>VLOOKUP($B11,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B11,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5869775.2079999996</v>
       </c>
       <c r="H11" s="22">
@@ -15276,7 +15330,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="20">
         <v>43433</v>
       </c>
@@ -15293,11 +15347,11 @@
         <v>198</v>
       </c>
       <c r="F12" s="12">
-        <f>VLOOKUP($B12,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B12,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>561224.13289999997</v>
       </c>
       <c r="G12" s="12">
-        <f>VLOOKUP($B12,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B12,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5870576.6859999998</v>
       </c>
       <c r="H12" s="22">
@@ -15322,7 +15376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="20">
         <v>43418</v>
       </c>
@@ -15339,11 +15393,11 @@
         <v>188</v>
       </c>
       <c r="F13" s="12">
-        <f>VLOOKUP($B13,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B13,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>436430.4179</v>
       </c>
       <c r="G13" s="12">
-        <f>VLOOKUP($B13,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B13,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5902814.034</v>
       </c>
       <c r="H13" s="22">
@@ -15368,7 +15422,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
         <v>43418</v>
       </c>
@@ -15385,11 +15439,11 @@
         <v>188</v>
       </c>
       <c r="F14" s="12">
-        <f>VLOOKUP($B14,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B14,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>437493.6974</v>
       </c>
       <c r="G14" s="12">
-        <f>VLOOKUP($B14,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B14,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5902547.2589999996</v>
       </c>
       <c r="H14" s="22">
@@ -15414,7 +15468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="20">
         <v>43418</v>
       </c>
@@ -15431,11 +15485,11 @@
         <v>188</v>
       </c>
       <c r="F15" s="12">
-        <f>VLOOKUP($B15,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B15,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>440397.66649999999</v>
       </c>
       <c r="G15" s="12">
-        <f>VLOOKUP($B15,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B15,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5901292.0489999996</v>
       </c>
       <c r="H15" s="22">
@@ -15460,7 +15514,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="20">
         <v>43419</v>
       </c>
@@ -15477,11 +15531,11 @@
         <v>188</v>
       </c>
       <c r="F16" s="12">
-        <f>VLOOKUP($B16,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B16,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>442776.59759999998</v>
       </c>
       <c r="G16" s="12">
-        <f>VLOOKUP($B16,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B16,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5899051.3799999999</v>
       </c>
       <c r="H16" s="22">
@@ -15506,7 +15560,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="20">
         <v>43419</v>
       </c>
@@ -15523,11 +15577,11 @@
         <v>198</v>
       </c>
       <c r="F17" s="12">
-        <f>VLOOKUP($B17,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B17,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>556685</v>
       </c>
       <c r="G17" s="12">
-        <f>VLOOKUP($B17,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B17,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5866808</v>
       </c>
       <c r="H17" s="22">
@@ -15552,7 +15606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="20">
         <v>43419</v>
       </c>
@@ -15569,11 +15623,11 @@
         <v>198</v>
       </c>
       <c r="F18" s="12">
-        <f>VLOOKUP($B18,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B18,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>556270</v>
       </c>
       <c r="G18" s="12">
-        <f>VLOOKUP($B18,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B18,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5867962</v>
       </c>
       <c r="H18" s="22">
@@ -15598,7 +15652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="20">
         <v>43419</v>
       </c>
@@ -15615,11 +15669,11 @@
         <v>188</v>
       </c>
       <c r="F19" s="12">
-        <f>VLOOKUP($B19,[1]Scat_coords_final!$A$2:$H$114,6,FALSE)</f>
+        <f>VLOOKUP($B19,[1]Scat_coords_final!$A$2:$H$117,6,FALSE)</f>
         <v>441778</v>
       </c>
       <c r="G19" s="12">
-        <f>VLOOKUP($B19,[1]Scat_coords_final!$A$2:$H$114,7,FALSE)</f>
+        <f>VLOOKUP($B19,[1]Scat_coords_final!$A$2:$H$117,7,FALSE)</f>
         <v>5905117</v>
       </c>
       <c r="H19" s="22">
@@ -15644,7 +15698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -15668,7 +15722,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15676,31 +15729,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0FB03E-0A2A-48C3-A625-3B810ED32825}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -15708,7 +15761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
Added trapping matrix for Swifts creek
</commit_message>
<xml_diff>
--- a/Data/TrappingSimulation.xlsx
+++ b/Data/TrappingSimulation.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Dropbox\Wild dogs\Forensics\Field work\Scat searches\TrappingSimulationAnalysis\WDTrappingAnalysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD783003-4BD1-4416-8051-E41D5CDFC46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EEF443-02E1-459B-B628-9AC883F70D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{2710E8AD-00DC-40F3-B0B0-9BC2CF75077C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2710E8AD-00DC-40F3-B0B0-9BC2CF75077C}"/>
   </bookViews>
   <sheets>
     <sheet name="Trap" sheetId="1" r:id="rId1"/>
     <sheet name="Matches" sheetId="3" r:id="rId2"/>
     <sheet name="Coords" sheetId="2" r:id="rId3"/>
-    <sheet name="Scats" sheetId="4" r:id="rId4"/>
-    <sheet name="Notes" sheetId="5" r:id="rId5"/>
+    <sheet name="Trap_SwiftsCreek" sheetId="6" r:id="rId4"/>
+    <sheet name="Scats" sheetId="4" r:id="rId5"/>
+    <sheet name="Notes" sheetId="5" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Coords!$A$1:$I$100</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Scats!$A$1:$N$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Scats!$A$1:$N$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="242">
   <si>
     <t xml:space="preserve">Day 1 </t>
   </si>
@@ -714,6 +715,81 @@
   </si>
   <si>
     <t>coords are now correct, see email from Luke (canidae) 01 Nov 2019</t>
+  </si>
+  <si>
+    <t>Trap Name</t>
+  </si>
+  <si>
+    <t>Day 69</t>
+  </si>
+  <si>
+    <t>Day 70</t>
+  </si>
+  <si>
+    <t>Day 71</t>
+  </si>
+  <si>
+    <t>Day 72</t>
+  </si>
+  <si>
+    <t>Day 73</t>
+  </si>
+  <si>
+    <t>Day 74</t>
+  </si>
+  <si>
+    <t>Day 75</t>
+  </si>
+  <si>
+    <t>Day 76</t>
+  </si>
+  <si>
+    <t>Day 77</t>
+  </si>
+  <si>
+    <t>Day 78</t>
+  </si>
+  <si>
+    <t>Trap 1</t>
+  </si>
+  <si>
+    <t>Trap 2</t>
+  </si>
+  <si>
+    <t>Trap 3</t>
+  </si>
+  <si>
+    <t>Trap 4</t>
+  </si>
+  <si>
+    <t>Trap 5</t>
+  </si>
+  <si>
+    <t>Trap 6</t>
+  </si>
+  <si>
+    <t>Trap 7</t>
+  </si>
+  <si>
+    <t>Trap 8</t>
+  </si>
+  <si>
+    <t>Trap 9</t>
+  </si>
+  <si>
+    <t>Trap 10</t>
+  </si>
+  <si>
+    <t>Trap 11</t>
+  </si>
+  <si>
+    <t>Trap 12</t>
+  </si>
+  <si>
+    <t>Trap 14</t>
+  </si>
+  <si>
+    <t>All the detection in Swift Creek trapping data were substitute with 0 to calculate trap effort</t>
   </si>
 </sst>
 </file>
@@ -796,7 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -859,12 +935,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1" xr:uid="{1CECCCD3-C251-429C-81B8-AD81D07AB5FD}"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -882,6 +961,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5795,9 +5888,9 @@
   <dimension ref="A1:CA110"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="AH1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="W11" sqref="W11"/>
+      <selection pane="topRight" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12086,12 +12179,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B31:AA31 B30:D30 F30:I30 L30:AA30 B33:AA107 B32:M32 O32:AA32 B109:AA109 B108:H108 J108:AA108 B10:BF14 BG10:CA10 B3:BZ4 BG11:BZ14 BG8:BR9 B3:BG10 BH15:BZ17 B20:AA29">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="BT8">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="BT8">
       <formula>NOT(ISERROR(SEARCH("BT8",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:BG19">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="BT8">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="BT8">
       <formula>NOT(ISERROR(SEARCH("BT8",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12185,7 +12278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC74EFC9-D6BB-4BDC-9373-237FF6938D88}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
@@ -14801,11 +14894,3220 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563D80C9-1D7C-4876-811C-515257A2EF82}">
+  <dimension ref="A1:BL103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AR1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A22" sqref="A22"/>
+      <selection pane="topRight" activeCell="BL4" sqref="BL4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="33" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="42" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.54296875" style="2" customWidth="1"/>
+    <col min="44" max="64" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="65" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4">
+        <v>43434</v>
+      </c>
+      <c r="C2" s="4">
+        <v>43435</v>
+      </c>
+      <c r="D2" s="4">
+        <v>43436</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43437</v>
+      </c>
+      <c r="F2" s="4">
+        <v>43438</v>
+      </c>
+      <c r="G2" s="4">
+        <v>43439</v>
+      </c>
+      <c r="H2" s="4">
+        <v>43440</v>
+      </c>
+      <c r="I2" s="4">
+        <v>43441</v>
+      </c>
+      <c r="J2" s="4">
+        <v>43442</v>
+      </c>
+      <c r="K2" s="4">
+        <v>43443</v>
+      </c>
+      <c r="L2" s="4">
+        <v>43444</v>
+      </c>
+      <c r="M2" s="4">
+        <v>43445</v>
+      </c>
+      <c r="N2" s="4">
+        <v>43446</v>
+      </c>
+      <c r="O2" s="4">
+        <v>43447</v>
+      </c>
+      <c r="P2" s="4">
+        <v>43448</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>43449</v>
+      </c>
+      <c r="R2" s="4">
+        <v>43450</v>
+      </c>
+      <c r="S2" s="4">
+        <v>43451</v>
+      </c>
+      <c r="T2" s="4">
+        <v>43452</v>
+      </c>
+      <c r="U2" s="4">
+        <v>43453</v>
+      </c>
+      <c r="V2" s="4">
+        <v>43454</v>
+      </c>
+      <c r="W2" s="4">
+        <v>43455</v>
+      </c>
+      <c r="X2" s="4">
+        <v>43456</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>43457</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>43458</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>43459</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>43460</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>43461</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>43462</v>
+      </c>
+      <c r="AE2" s="4">
+        <v>43463</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>43464</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>43465</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>43466</v>
+      </c>
+      <c r="AI2" s="4">
+        <v>43467</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>43468</v>
+      </c>
+      <c r="AK2" s="4">
+        <v>43469</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>43470</v>
+      </c>
+      <c r="AM2" s="4">
+        <v>43471</v>
+      </c>
+      <c r="AN2" s="4">
+        <v>43472</v>
+      </c>
+      <c r="AO2" s="4">
+        <v>43473</v>
+      </c>
+      <c r="AP2" s="4">
+        <v>43474</v>
+      </c>
+      <c r="AQ2" s="4">
+        <v>43475</v>
+      </c>
+      <c r="AR2" s="4">
+        <v>43476</v>
+      </c>
+      <c r="AS2" s="4">
+        <v>43477</v>
+      </c>
+      <c r="AT2" s="4">
+        <v>43478</v>
+      </c>
+      <c r="AU2" s="4">
+        <v>43479</v>
+      </c>
+      <c r="AV2" s="4">
+        <v>43480</v>
+      </c>
+      <c r="AW2" s="4">
+        <v>43481</v>
+      </c>
+      <c r="AX2" s="4">
+        <v>43482</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>43483</v>
+      </c>
+      <c r="AZ2" s="4">
+        <v>43484</v>
+      </c>
+      <c r="BA2" s="4">
+        <v>43485</v>
+      </c>
+      <c r="BB2" s="4">
+        <v>43486</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>43487</v>
+      </c>
+      <c r="BD2" s="4">
+        <v>43488</v>
+      </c>
+      <c r="BE2" s="4">
+        <v>43489</v>
+      </c>
+      <c r="BF2" s="4">
+        <v>43490</v>
+      </c>
+      <c r="BG2" s="4">
+        <v>43491</v>
+      </c>
+      <c r="BH2" s="4">
+        <v>43492</v>
+      </c>
+      <c r="BI2" s="4">
+        <v>43493</v>
+      </c>
+      <c r="BJ2" s="4">
+        <v>43494</v>
+      </c>
+      <c r="BK2" s="4">
+        <v>43495</v>
+      </c>
+      <c r="BL2" s="4">
+        <v>43496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL3" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2">
+        <v>0</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2">
+        <v>0</v>
+      </c>
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2">
+        <v>0</v>
+      </c>
+      <c r="W10" s="2">
+        <v>0</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL11" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
+        <v>0</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL14" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0</v>
+      </c>
+      <c r="V15" s="2">
+        <v>0</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BE15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BG15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A62" s="1"/>
+      <c r="W62" s="26"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" s="1"/>
+      <c r="D89" s="26"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="1"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B25:AA25 B24:D24 F24:I24 L24:AA24 B27:AA101 B26:M26 O26:AA26 B103:AA103 B102:H102 J102:AA102 B6:AO6 B7:U8 W7:AO7 B9:BB10 B5:AU5 B16:AA23 B3:BL4 BC10:BM10 BC9:BD9 W8:BD8 B11:BL15">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="BT8">
+      <formula>NOT(ISERROR(SEARCH("BT8",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V7:V8">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="BT8">
+      <formula>NOT(ISERROR(SEARCH("BT8",V7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FCDAD8-3241-4B9B-A741-CC3F8E4D1679}">
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15725,12 +19027,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0FB03E-0A2A-48C3-A625-3B810ED32825}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15769,6 +19071,11 @@
         <v>216</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>241</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>